<commit_message>
add activities attached to an account
</commit_message>
<xml_diff>
--- a/pipeline_updates.xlsx
+++ b/pipeline_updates.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gjung18/Workspace/emd/emd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE67D80-F980-ED4A-8F5B-1937C71359D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CCD7A7-C7FB-A04E-88C3-78577A4E9C43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30500" windowHeight="16920" activeTab="1" xr2:uid="{95744BB1-B1C7-41ED-B352-8C3E88B99EF1}"/>
+    <workbookView xWindow="3100" yWindow="1700" windowWidth="30500" windowHeight="16920" xr2:uid="{95744BB1-B1C7-41ED-B352-8C3E88B99EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Pipeline" sheetId="1" r:id="rId1"/>
-    <sheet name="Opp" sheetId="2" r:id="rId2"/>
+    <sheet name="Account Updates" sheetId="3" r:id="rId2"/>
+    <sheet name="Opp" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Meeting:</t>
   </si>
@@ -161,6 +162,21 @@
   </si>
   <si>
     <t>beta.SAM.gov Link:</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -278,8 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -296,7 +310,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -659,29 +679,27 @@
   </sheetPr>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
     <col min="6" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="14"/>
@@ -697,10 +715,10 @@
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="13"/>
-      <c r="M1" s="9"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="14"/>
@@ -716,10 +734,10 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="13"/>
-      <c r="M2" s="9"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="14"/>
@@ -735,10 +753,10 @@
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="13"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -771,7 +789,7 @@
       <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1031,14 +1049,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A36D41F-F55B-1542-B79D-43C4BCB344C1}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90032EBE-9927-4331-8EED-543F0FCC6CD1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:D16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1059,27 +1116,27 @@
       <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="19"/>
@@ -1087,7 +1144,7 @@
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="19"/>
@@ -1095,7 +1152,7 @@
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="19"/>
@@ -1103,7 +1160,7 @@
       <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="11"/>
@@ -1111,84 +1168,84 @@
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">

</xml_diff>